<commit_message>
Basic geometry and neighbors measures. Also updating Rakefile update_resources task to update files according to a csv file.
</commit_message>
<xml_diff>
--- a/OpenStudio-analysis-spreadsheet/projects/003Phoenix_2story_1800_Slab_UA_Grg.xlsx
+++ b/OpenStudio-analysis-spreadsheet/projects/003Phoenix_2story_1800_Slab_UA_Grg.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3568" uniqueCount="1253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3593" uniqueCount="1253">
   <si>
     <t>type</t>
   </si>
@@ -3643,9 +3643,6 @@
     <t>Slab Perimeter</t>
   </si>
   <si>
-    <t>Partition Wall Mass: Num Layers</t>
-  </si>
-  <si>
     <t>U-Value</t>
   </si>
   <si>
@@ -3800,6 +3797,9 @@
   </si>
   <si>
     <t>Garage Area</t>
+  </si>
+  <si>
+    <t>ProcessConstructionsInteriorUninsulatedWalls</t>
   </si>
 </sst>
 </file>
@@ -5943,12 +5943,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -8086,8 +8086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8439,7 +8439,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D37" s="2"/>
     </row>
@@ -8521,11 +8521,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z336"/>
+  <dimension ref="A1:Z342"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A146" sqref="A146"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8581,14 +8581,14 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="70" t="s">
+      <c r="U1" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
+      <c r="V1" s="73"/>
+      <c r="W1" s="73"/>
+      <c r="X1" s="73"/>
+      <c r="Y1" s="73"/>
+      <c r="Z1" s="73"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -9877,7 +9877,7 @@
         <v>21</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="E68" s="31" t="s">
         <v>908</v>
@@ -9894,10 +9894,10 @@
         <v>21</v>
       </c>
       <c r="D69" s="31" t="s">
+        <v>1248</v>
+      </c>
+      <c r="E69" s="31" t="s">
         <v>1249</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>1250</v>
       </c>
       <c r="G69" s="31" t="s">
         <v>64</v>
@@ -9911,10 +9911,10 @@
         <v>21</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="G70" s="31" t="s">
         <v>64</v>
@@ -10161,7 +10161,7 @@
       <c r="G84" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I84" s="71" t="s">
+      <c r="I84" s="70" t="s">
         <v>1165</v>
       </c>
     </row>
@@ -12147,7 +12147,7 @@
         <v>64</v>
       </c>
       <c r="I198" s="46" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="J198" s="31"/>
       <c r="K198" s="46"/>
@@ -12170,7 +12170,7 @@
         <v>64</v>
       </c>
       <c r="I199" s="46" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="J199" s="31"/>
       <c r="K199" s="46"/>
@@ -12234,7 +12234,7 @@
         <v>21</v>
       </c>
       <c r="D203" s="31" t="s">
-        <v>1149</v>
+        <v>1144</v>
       </c>
       <c r="E203" s="31" t="s">
         <v>859</v>
@@ -12251,7 +12251,7 @@
         <v>21</v>
       </c>
       <c r="D204" s="31" t="s">
-        <v>1200</v>
+        <v>1145</v>
       </c>
       <c r="E204" s="31" t="s">
         <v>860</v>
@@ -12370,71 +12370,69 @@
         <v>1</v>
       </c>
       <c r="B211" s="47" t="s">
-        <v>723</v>
+        <v>1252</v>
       </c>
       <c r="C211" s="47" t="s">
-        <v>723</v>
+        <v>1252</v>
       </c>
       <c r="D211" s="47" t="s">
-        <v>723</v>
+        <v>1252</v>
       </c>
       <c r="E211" s="48" t="s">
         <v>68</v>
       </c>
+      <c r="H211" s="49"/>
       <c r="I211" s="49"/>
-      <c r="J211" s="49"/>
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B212" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D212" s="31" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="E212" s="31" t="s">
-        <v>889</v>
+        <v>707</v>
       </c>
       <c r="G212" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I212" s="4" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="B213" s="47" t="s">
-        <v>1244</v>
-      </c>
-      <c r="C213" s="47" t="s">
-        <v>1244</v>
-      </c>
-      <c r="D213" s="47" t="s">
-        <v>1244</v>
-      </c>
-      <c r="E213" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="I213" s="49"/>
-      <c r="J213" s="49"/>
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B213" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D213" s="31" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E213" s="31" t="s">
+        <v>890</v>
+      </c>
+      <c r="G213" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I213" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B214" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D214" s="31" t="s">
-        <v>1123</v>
+        <v>1150</v>
       </c>
       <c r="E214" s="31" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="G214" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I214" s="4" t="s">
-        <v>1051</v>
+        <v>64</v>
+      </c>
+      <c r="I214" s="4">
+        <v>1.1112</v>
       </c>
     </row>
     <row r="215" spans="1:10" x14ac:dyDescent="0.25">
@@ -12442,16 +12440,16 @@
         <v>21</v>
       </c>
       <c r="D215" s="31" t="s">
-        <v>1137</v>
-      </c>
-      <c r="E215" s="72" t="s">
-        <v>886</v>
+        <v>1151</v>
+      </c>
+      <c r="E215" s="31" t="s">
+        <v>892</v>
       </c>
       <c r="G215" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I215" s="4" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="I215" s="4">
+        <v>50</v>
       </c>
     </row>
     <row r="216" spans="1:10" x14ac:dyDescent="0.25">
@@ -12459,86 +12457,88 @@
         <v>21</v>
       </c>
       <c r="D216" s="31" t="s">
-        <v>1146</v>
+        <v>1152</v>
       </c>
       <c r="E216" s="31" t="s">
-        <v>887</v>
+        <v>893</v>
       </c>
       <c r="G216" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I216" s="4">
-        <v>0.91</v>
-      </c>
-    </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B217" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D217" s="31" t="s">
-        <v>1147</v>
-      </c>
-      <c r="E217" s="72" t="s">
-        <v>888</v>
-      </c>
-      <c r="G217" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I217" s="4">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="218" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="47" t="b">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="B218" s="47" t="s">
-        <v>724</v>
-      </c>
-      <c r="C218" s="47" t="s">
-        <v>724</v>
-      </c>
-      <c r="D218" s="47" t="s">
-        <v>724</v>
-      </c>
-      <c r="E218" s="48" t="s">
+      <c r="B217" s="47" t="s">
+        <v>723</v>
+      </c>
+      <c r="C217" s="47" t="s">
+        <v>723</v>
+      </c>
+      <c r="D217" s="47" t="s">
+        <v>723</v>
+      </c>
+      <c r="E217" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="I218" s="49"/>
-      <c r="J218" s="49"/>
-    </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B219" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D219" s="31" t="s">
-        <v>1201</v>
-      </c>
-      <c r="E219" s="31" t="s">
-        <v>902</v>
-      </c>
-      <c r="G219" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I219" s="4">
-        <v>0.37</v>
-      </c>
+      <c r="I217" s="49"/>
+      <c r="J217" s="49"/>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B218" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D218" s="31" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E218" s="31" t="s">
+        <v>889</v>
+      </c>
+      <c r="G218" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I218" s="4" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B219" s="47" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C219" s="47" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D219" s="47" t="s">
+        <v>1243</v>
+      </c>
+      <c r="E219" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I219" s="49"/>
+      <c r="J219" s="49"/>
     </row>
     <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B220" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D220" s="31" t="s">
-        <v>901</v>
+        <v>1123</v>
       </c>
       <c r="E220" s="31" t="s">
-        <v>903</v>
+        <v>889</v>
       </c>
       <c r="G220" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I220" s="4">
-        <v>0.3</v>
+        <v>62</v>
+      </c>
+      <c r="I220" s="4" t="s">
+        <v>1051</v>
       </c>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
@@ -12546,16 +12546,16 @@
         <v>21</v>
       </c>
       <c r="D221" s="31" t="s">
-        <v>1202</v>
-      </c>
-      <c r="E221" s="31" t="s">
-        <v>904</v>
+        <v>1137</v>
+      </c>
+      <c r="E221" s="71" t="s">
+        <v>886</v>
       </c>
       <c r="G221" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I221" s="4">
-        <v>0.7</v>
+        <v>63</v>
+      </c>
+      <c r="I221" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:10" x14ac:dyDescent="0.25">
@@ -12563,326 +12563,328 @@
         <v>21</v>
       </c>
       <c r="D222" s="31" t="s">
-        <v>1203</v>
+        <v>1146</v>
       </c>
       <c r="E222" s="31" t="s">
-        <v>905</v>
+        <v>887</v>
       </c>
       <c r="G222" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I222" s="4">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="223" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="47" t="b">
-        <v>1</v>
-      </c>
-      <c r="B223" s="47" t="s">
-        <v>1008</v>
-      </c>
-      <c r="C223" s="47" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D223" s="47" t="s">
-        <v>1008</v>
-      </c>
-      <c r="E223" s="48" t="s">
-        <v>160</v>
-      </c>
-      <c r="I223" s="49"/>
-      <c r="J223" s="49"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B223" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D223" s="31" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E223" s="71" t="s">
+        <v>888</v>
+      </c>
+      <c r="G223" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I223" s="4">
+        <v>0.85</v>
+      </c>
     </row>
     <row r="224" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A224" s="47" t="b">
         <v>1</v>
       </c>
       <c r="B224" s="47" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="C224" s="47" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="D224" s="47" t="s">
-        <v>731</v>
+        <v>724</v>
       </c>
       <c r="E224" s="48" t="s">
-        <v>160</v>
+        <v>68</v>
       </c>
       <c r="I224" s="49"/>
       <c r="J224" s="49"/>
     </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B225" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D225" s="31" t="s">
+        <v>1200</v>
+      </c>
+      <c r="E225" s="31" t="s">
+        <v>902</v>
+      </c>
+      <c r="G225" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I225" s="4">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B226" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D226" s="31" t="s">
+        <v>901</v>
+      </c>
+      <c r="E226" s="31" t="s">
+        <v>903</v>
+      </c>
+      <c r="G226" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I226" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B227" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D227" s="31" t="s">
+        <v>1201</v>
+      </c>
+      <c r="E227" s="31" t="s">
+        <v>904</v>
+      </c>
+      <c r="G227" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I227" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B228" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D228" s="31" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E228" s="31" t="s">
+        <v>905</v>
+      </c>
+      <c r="G228" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I228" s="4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B229" s="47" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C229" s="47" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D229" s="47" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E229" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="I229" s="49"/>
+      <c r="J229" s="49"/>
+    </row>
+    <row r="230" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="47" t="b">
+        <v>1</v>
+      </c>
+      <c r="B230" s="47" t="s">
+        <v>731</v>
+      </c>
+      <c r="C230" s="47" t="s">
+        <v>731</v>
+      </c>
+      <c r="D230" s="47" t="s">
+        <v>731</v>
+      </c>
+      <c r="E230" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="I230" s="49"/>
+      <c r="J230" s="49"/>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B231" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D231" s="31" t="s">
         <v>1121</v>
       </c>
-      <c r="E225" s="31" t="s">
+      <c r="E231" s="31" t="s">
         <v>707</v>
       </c>
-      <c r="G225" s="31" t="s">
+      <c r="G231" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I225" s="4" t="s">
+      <c r="I231" s="4" t="s">
         <v>1175</v>
       </c>
     </row>
-    <row r="226" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B226" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D226" s="31" t="s">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B232" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" s="31" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E232" s="31" t="s">
+        <v>924</v>
+      </c>
+      <c r="G232" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I232" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B233" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D233" s="31" t="s">
         <v>1204</v>
       </c>
-      <c r="E226" s="31" t="s">
-        <v>924</v>
-      </c>
-      <c r="G226" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I226" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B227" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D227" s="31" t="s">
+      <c r="E233" s="31" t="s">
+        <v>925</v>
+      </c>
+      <c r="G233" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I233" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B234" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D234" s="31" t="s">
         <v>1205</v>
       </c>
-      <c r="E227" s="31" t="s">
-        <v>925</v>
-      </c>
-      <c r="G227" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I227" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="228" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B228" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D228" s="31" t="s">
+      <c r="E234" s="31" t="s">
+        <v>926</v>
+      </c>
+      <c r="G234" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="I234" s="4" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B235" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D235" s="31" t="s">
         <v>1206</v>
       </c>
-      <c r="E228" s="31" t="s">
-        <v>926</v>
-      </c>
-      <c r="G228" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I228" s="4" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="229" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B229" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D229" s="31" t="s">
+      <c r="E235" s="31" t="s">
+        <v>889</v>
+      </c>
+      <c r="G235" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I235" s="4" t="s">
         <v>1207</v>
       </c>
-      <c r="E229" s="31" t="s">
-        <v>889</v>
-      </c>
-      <c r="G229" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I229" s="4" t="s">
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B236" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D236" s="31" t="s">
         <v>1208</v>
       </c>
-    </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B230" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D230" s="31" t="s">
-        <v>1209</v>
-      </c>
-      <c r="E230" s="31" t="s">
+      <c r="E236" s="31" t="s">
         <v>894</v>
-      </c>
-      <c r="G230" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I230" s="4" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="231" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B231" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D231" s="31" t="s">
-        <v>1210</v>
-      </c>
-      <c r="E231" s="31" t="s">
-        <v>927</v>
-      </c>
-      <c r="G231" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I231" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="232" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B232" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D232" s="31" t="s">
-        <v>1211</v>
-      </c>
-      <c r="E232" s="31" t="s">
-        <v>909</v>
-      </c>
-      <c r="G232" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I232" s="4" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="233" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B233" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D233" s="31" t="s">
-        <v>1212</v>
-      </c>
-      <c r="E233" s="31" t="s">
-        <v>930</v>
-      </c>
-      <c r="G233" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I233" s="4">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B234" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D234" s="31" t="s">
-        <v>1213</v>
-      </c>
-      <c r="E234" s="31" t="s">
-        <v>931</v>
-      </c>
-      <c r="G234" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I234" s="4" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="235" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B235" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D235" s="31" t="s">
-        <v>1214</v>
-      </c>
-      <c r="E235" s="31" t="s">
-        <v>932</v>
-      </c>
-      <c r="G235" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I235" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="236" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B236" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D236" s="31" t="s">
-        <v>1215</v>
-      </c>
-      <c r="E236" s="31" t="s">
-        <v>933</v>
       </c>
       <c r="G236" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I236" s="4" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.25">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B237" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D237" s="31" t="s">
-        <v>1217</v>
+        <v>1209</v>
       </c>
       <c r="E237" s="31" t="s">
-        <v>934</v>
+        <v>927</v>
       </c>
       <c r="G237" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I237" s="4">
-        <v>3.3300000000000001E-3</v>
-      </c>
-    </row>
-    <row r="238" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B238" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D238" s="31" t="s">
-        <v>1218</v>
+        <v>1210</v>
       </c>
       <c r="E238" s="31" t="s">
-        <v>935</v>
+        <v>909</v>
       </c>
       <c r="G238" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I238" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="I238" s="4" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B239" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D239" s="31" t="s">
-        <v>1219</v>
+        <v>1211</v>
       </c>
       <c r="E239" s="31" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="G239" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I239" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="240" spans="2:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B240" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D240" s="31" t="s">
-        <v>1220</v>
+        <v>1212</v>
       </c>
       <c r="E240" s="31" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="G240" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I240" s="4" t="s">
-        <v>938</v>
+        <v>929</v>
       </c>
     </row>
     <row r="241" spans="2:9" x14ac:dyDescent="0.25">
@@ -12890,16 +12892,16 @@
         <v>21</v>
       </c>
       <c r="D241" s="31" t="s">
-        <v>1221</v>
+        <v>1213</v>
       </c>
       <c r="E241" s="31" t="s">
-        <v>939</v>
+        <v>932</v>
       </c>
       <c r="G241" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I241" s="4" t="s">
-        <v>1229</v>
+        <v>64</v>
+      </c>
+      <c r="I241" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.25">
@@ -12907,16 +12909,16 @@
         <v>21</v>
       </c>
       <c r="D242" s="31" t="s">
-        <v>1222</v>
+        <v>1214</v>
       </c>
       <c r="E242" s="31" t="s">
-        <v>940</v>
+        <v>933</v>
       </c>
       <c r="G242" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I242" s="4" t="b">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="I242" s="4" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.25">
@@ -12924,16 +12926,16 @@
         <v>21</v>
       </c>
       <c r="D243" s="31" t="s">
-        <v>1223</v>
+        <v>1216</v>
       </c>
       <c r="E243" s="31" t="s">
-        <v>941</v>
+        <v>934</v>
       </c>
       <c r="G243" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I243" s="4">
-        <v>0</v>
+        <v>3.3300000000000001E-3</v>
       </c>
     </row>
     <row r="244" spans="2:9" x14ac:dyDescent="0.25">
@@ -12941,10 +12943,10 @@
         <v>21</v>
       </c>
       <c r="D244" s="31" t="s">
-        <v>1224</v>
+        <v>1217</v>
       </c>
       <c r="E244" s="31" t="s">
-        <v>942</v>
+        <v>935</v>
       </c>
       <c r="G244" s="31" t="s">
         <v>64</v>
@@ -12958,16 +12960,16 @@
         <v>21</v>
       </c>
       <c r="D245" s="31" t="s">
-        <v>1225</v>
+        <v>1218</v>
       </c>
       <c r="E245" s="31" t="s">
-        <v>943</v>
+        <v>936</v>
       </c>
       <c r="G245" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I245" s="4">
-        <v>1.0000000000000001E-5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246" spans="2:9" x14ac:dyDescent="0.25">
@@ -12975,16 +12977,16 @@
         <v>21</v>
       </c>
       <c r="D246" s="31" t="s">
-        <v>1226</v>
+        <v>1219</v>
       </c>
       <c r="E246" s="31" t="s">
-        <v>944</v>
+        <v>937</v>
       </c>
       <c r="G246" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I246" s="4">
-        <v>1.0000000000000001E-5</v>
+        <v>62</v>
+      </c>
+      <c r="I246" s="4" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.25">
@@ -12992,16 +12994,16 @@
         <v>21</v>
       </c>
       <c r="D247" s="31" t="s">
-        <v>1227</v>
+        <v>1220</v>
       </c>
       <c r="E247" s="31" t="s">
-        <v>1228</v>
+        <v>939</v>
       </c>
       <c r="G247" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I247" s="73" t="s">
-        <v>1245</v>
+      <c r="I247" s="4" t="s">
+        <v>1228</v>
       </c>
     </row>
     <row r="248" spans="2:9" x14ac:dyDescent="0.25">
@@ -13009,16 +13011,16 @@
         <v>21</v>
       </c>
       <c r="D248" s="31" t="s">
-        <v>1230</v>
+        <v>1221</v>
       </c>
       <c r="E248" s="31" t="s">
-        <v>945</v>
+        <v>940</v>
       </c>
       <c r="G248" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I248" s="4">
-        <v>100</v>
+        <v>63</v>
+      </c>
+      <c r="I248" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="2:9" x14ac:dyDescent="0.25">
@@ -13026,10 +13028,10 @@
         <v>21</v>
       </c>
       <c r="D249" s="31" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="E249" s="31" t="s">
-        <v>971</v>
+        <v>941</v>
       </c>
       <c r="G249" s="31" t="s">
         <v>64</v>
@@ -13043,10 +13045,10 @@
         <v>21</v>
       </c>
       <c r="D250" s="31" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="E250" s="31" t="s">
-        <v>972</v>
+        <v>942</v>
       </c>
       <c r="G250" s="31" t="s">
         <v>64</v>
@@ -13060,16 +13062,16 @@
         <v>21</v>
       </c>
       <c r="D251" s="31" t="s">
-        <v>1233</v>
+        <v>1224</v>
       </c>
       <c r="E251" s="31" t="s">
-        <v>973</v>
+        <v>943</v>
       </c>
       <c r="G251" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I251" s="4">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="252" spans="2:9" x14ac:dyDescent="0.25">
@@ -13077,16 +13079,16 @@
         <v>21</v>
       </c>
       <c r="D252" s="31" t="s">
-        <v>1234</v>
+        <v>1225</v>
       </c>
       <c r="E252" s="31" t="s">
-        <v>974</v>
+        <v>944</v>
       </c>
       <c r="G252" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I252" s="4" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="I252" s="4">
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.25">
@@ -13094,16 +13096,16 @@
         <v>21</v>
       </c>
       <c r="D253" s="31" t="s">
-        <v>1235</v>
+        <v>1226</v>
       </c>
       <c r="E253" s="31" t="s">
-        <v>975</v>
+        <v>1227</v>
       </c>
       <c r="G253" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I253" s="4" t="b">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="I253" s="72" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="254" spans="2:9" x14ac:dyDescent="0.25">
@@ -13111,16 +13113,16 @@
         <v>21</v>
       </c>
       <c r="D254" s="31" t="s">
-        <v>1236</v>
+        <v>1229</v>
       </c>
       <c r="E254" s="31" t="s">
-        <v>976</v>
+        <v>945</v>
       </c>
       <c r="G254" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I254" s="4" t="b">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="I254" s="4">
+        <v>100</v>
       </c>
     </row>
     <row r="255" spans="2:9" x14ac:dyDescent="0.25">
@@ -13128,10 +13130,10 @@
         <v>21</v>
       </c>
       <c r="D255" s="31" t="s">
-        <v>1237</v>
+        <v>1230</v>
       </c>
       <c r="E255" s="31" t="s">
-        <v>977</v>
+        <v>971</v>
       </c>
       <c r="G255" s="31" t="s">
         <v>64</v>
@@ -13145,10 +13147,10 @@
         <v>21</v>
       </c>
       <c r="D256" s="31" t="s">
-        <v>1238</v>
+        <v>1231</v>
       </c>
       <c r="E256" s="31" t="s">
-        <v>978</v>
+        <v>972</v>
       </c>
       <c r="G256" s="31" t="s">
         <v>64</v>
@@ -13162,10 +13164,10 @@
         <v>21</v>
       </c>
       <c r="D257" s="31" t="s">
-        <v>1239</v>
+        <v>1232</v>
       </c>
       <c r="E257" s="31" t="s">
-        <v>979</v>
+        <v>973</v>
       </c>
       <c r="G257" s="31" t="s">
         <v>64</v>
@@ -13179,15 +13181,15 @@
         <v>21</v>
       </c>
       <c r="D258" s="31" t="s">
-        <v>1240</v>
+        <v>1233</v>
       </c>
       <c r="E258" s="31" t="s">
-        <v>980</v>
+        <v>974</v>
       </c>
       <c r="G258" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I258" s="4">
+        <v>63</v>
+      </c>
+      <c r="I258" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -13196,15 +13198,15 @@
         <v>21</v>
       </c>
       <c r="D259" s="31" t="s">
-        <v>1241</v>
+        <v>1234</v>
       </c>
       <c r="E259" s="31" t="s">
-        <v>981</v>
+        <v>975</v>
       </c>
       <c r="G259" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I259" s="4">
+        <v>63</v>
+      </c>
+      <c r="I259" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -13213,15 +13215,15 @@
         <v>21</v>
       </c>
       <c r="D260" s="31" t="s">
-        <v>1242</v>
+        <v>1235</v>
       </c>
       <c r="E260" s="31" t="s">
-        <v>982</v>
+        <v>976</v>
       </c>
       <c r="G260" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I260" s="4">
+        <v>63</v>
+      </c>
+      <c r="I260" s="4" t="b">
         <v>0</v>
       </c>
     </row>
@@ -13230,16 +13232,16 @@
         <v>21</v>
       </c>
       <c r="D261" s="31" t="s">
-        <v>946</v>
+        <v>1236</v>
       </c>
       <c r="E261" s="31" t="s">
-        <v>983</v>
+        <v>977</v>
       </c>
       <c r="G261" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I261" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.25">
@@ -13247,16 +13249,16 @@
         <v>21</v>
       </c>
       <c r="D262" s="31" t="s">
-        <v>947</v>
+        <v>1237</v>
       </c>
       <c r="E262" s="31" t="s">
-        <v>984</v>
+        <v>978</v>
       </c>
       <c r="G262" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I262" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="2:9" x14ac:dyDescent="0.25">
@@ -13264,16 +13266,16 @@
         <v>21</v>
       </c>
       <c r="D263" s="31" t="s">
-        <v>948</v>
+        <v>1238</v>
       </c>
       <c r="E263" s="31" t="s">
-        <v>985</v>
+        <v>979</v>
       </c>
       <c r="G263" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I263" s="4">
-        <v>1828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.25">
@@ -13281,16 +13283,16 @@
         <v>21</v>
       </c>
       <c r="D264" s="31" t="s">
-        <v>949</v>
+        <v>1239</v>
       </c>
       <c r="E264" s="31" t="s">
-        <v>986</v>
+        <v>980</v>
       </c>
       <c r="G264" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I264" s="4">
-        <v>1828</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.25">
@@ -13298,16 +13300,16 @@
         <v>21</v>
       </c>
       <c r="D265" s="31" t="s">
-        <v>950</v>
+        <v>1240</v>
       </c>
       <c r="E265" s="31" t="s">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="G265" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I265" s="4">
-        <v>24.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="2:9" x14ac:dyDescent="0.25">
@@ -13315,16 +13317,16 @@
         <v>21</v>
       </c>
       <c r="D266" s="31" t="s">
-        <v>951</v>
+        <v>1241</v>
       </c>
       <c r="E266" s="31" t="s">
-        <v>988</v>
+        <v>982</v>
       </c>
       <c r="G266" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I266" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.25">
@@ -13332,16 +13334,16 @@
         <v>21</v>
       </c>
       <c r="D267" s="31" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="E267" s="31" t="s">
-        <v>989</v>
+        <v>983</v>
       </c>
       <c r="G267" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I267" s="4">
-        <v>266</v>
+        <v>3</v>
       </c>
     </row>
     <row r="268" spans="2:9" x14ac:dyDescent="0.25">
@@ -13349,16 +13351,16 @@
         <v>21</v>
       </c>
       <c r="D268" s="31" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="E268" s="31" t="s">
-        <v>990</v>
+        <v>984</v>
       </c>
       <c r="G268" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I268" s="4">
-        <v>14624</v>
+        <v>2</v>
       </c>
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.25">
@@ -13366,16 +13368,16 @@
         <v>21</v>
       </c>
       <c r="D269" s="31" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="E269" s="31" t="s">
-        <v>991</v>
+        <v>985</v>
       </c>
       <c r="G269" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I269" s="4">
-        <v>19.5</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.25">
@@ -13383,10 +13385,10 @@
         <v>21</v>
       </c>
       <c r="D270" s="31" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
       <c r="E270" s="31" t="s">
-        <v>992</v>
+        <v>986</v>
       </c>
       <c r="G270" s="31" t="s">
         <v>64</v>
@@ -13400,16 +13402,16 @@
         <v>21</v>
       </c>
       <c r="D271" s="31" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
       <c r="E271" s="31" t="s">
-        <v>993</v>
+        <v>987</v>
       </c>
       <c r="G271" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I271" s="4">
-        <v>3295.5</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="272" spans="2:9" x14ac:dyDescent="0.25">
@@ -13417,180 +13419,180 @@
         <v>21</v>
       </c>
       <c r="D272" s="31" t="s">
+        <v>951</v>
+      </c>
+      <c r="E272" s="31" t="s">
+        <v>988</v>
+      </c>
+      <c r="G272" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I272" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B273" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D273" s="31" t="s">
+        <v>952</v>
+      </c>
+      <c r="E273" s="31" t="s">
+        <v>989</v>
+      </c>
+      <c r="G273" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I273" s="4">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="274" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B274" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D274" s="31" t="s">
+        <v>953</v>
+      </c>
+      <c r="E274" s="31" t="s">
+        <v>990</v>
+      </c>
+      <c r="G274" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I274" s="4">
+        <v>14624</v>
+      </c>
+    </row>
+    <row r="275" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B275" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D275" s="31" t="s">
+        <v>954</v>
+      </c>
+      <c r="E275" s="31" t="s">
+        <v>991</v>
+      </c>
+      <c r="G275" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I275" s="4">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="276" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B276" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D276" s="31" t="s">
+        <v>955</v>
+      </c>
+      <c r="E276" s="31" t="s">
+        <v>992</v>
+      </c>
+      <c r="G276" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I276" s="4">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="277" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B277" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D277" s="31" t="s">
+        <v>956</v>
+      </c>
+      <c r="E277" s="31" t="s">
+        <v>993</v>
+      </c>
+      <c r="G277" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I277" s="4">
+        <v>3295.5</v>
+      </c>
+    </row>
+    <row r="278" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B278" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D278" s="31" t="s">
         <v>957</v>
       </c>
-      <c r="E272" s="31" t="s">
+      <c r="E278" s="31" t="s">
         <v>994</v>
       </c>
-      <c r="G272" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I272" s="4">
+      <c r="G278" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I278" s="4">
         <v>8.5</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B273" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D273" s="31" t="s">
+    <row r="279" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B279" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D279" s="31" t="s">
         <v>958</v>
       </c>
-      <c r="E273" s="31" t="s">
+      <c r="E279" s="31" t="s">
         <v>995</v>
       </c>
-      <c r="G273" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I273" s="4">
+      <c r="G279" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I279" s="4">
         <v>1014</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B274" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D274" s="31" t="s">
+    <row r="280" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B280" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D280" s="31" t="s">
         <v>959</v>
       </c>
-      <c r="E274" s="31" t="s">
+      <c r="E280" s="31" t="s">
         <v>996</v>
       </c>
-      <c r="G274" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I274" s="4">
+      <c r="G280" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I280" s="4">
         <v>4800</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B275" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D275" s="31" t="s">
+    <row r="281" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B281" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D281" s="31" t="s">
         <v>960</v>
       </c>
-      <c r="E275" s="31" t="s">
+      <c r="E281" s="31" t="s">
         <v>997</v>
       </c>
-      <c r="G275" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I275" s="4">
+      <c r="G281" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I281" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B276" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D276" s="31" t="s">
+    <row r="282" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B282" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D282" s="31" t="s">
         <v>961</v>
       </c>
-      <c r="E276" s="31" t="s">
+      <c r="E282" s="31" t="s">
         <v>998</v>
-      </c>
-      <c r="G276" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I276" s="4">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B277" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D277" s="31" t="s">
-        <v>962</v>
-      </c>
-      <c r="E277" s="31" t="s">
-        <v>999</v>
-      </c>
-      <c r="G277" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I277" s="4">
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B278" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D278" s="31" t="s">
-        <v>963</v>
-      </c>
-      <c r="E278" s="31" t="s">
-        <v>1000</v>
-      </c>
-      <c r="G278" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I278" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B279" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D279" s="31" t="s">
-        <v>964</v>
-      </c>
-      <c r="E279" s="31" t="s">
-        <v>1001</v>
-      </c>
-      <c r="G279" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I279" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B280" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D280" s="31" t="s">
-        <v>965</v>
-      </c>
-      <c r="E280" s="31" t="s">
-        <v>1002</v>
-      </c>
-      <c r="G280" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I280" s="4">
-        <v>9600</v>
-      </c>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B281" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D281" s="31" t="s">
-        <v>966</v>
-      </c>
-      <c r="E281" s="31" t="s">
-        <v>1003</v>
-      </c>
-      <c r="G281" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I281" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B282" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D282" s="31" t="s">
-        <v>967</v>
-      </c>
-      <c r="E282" s="31" t="s">
-        <v>1004</v>
       </c>
       <c r="G282" s="31" t="s">
         <v>64</v>
@@ -13599,32 +13601,32 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B283" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D283" s="31" t="s">
-        <v>968</v>
+        <v>962</v>
       </c>
       <c r="E283" s="31" t="s">
-        <v>1005</v>
+        <v>999</v>
       </c>
       <c r="G283" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I283" s="4">
-        <v>9600</v>
-      </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="284" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B284" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D284" s="31" t="s">
-        <v>969</v>
+        <v>963</v>
       </c>
       <c r="E284" s="31" t="s">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="G284" s="31" t="s">
         <v>64</v>
@@ -13633,71 +13635,72 @@
         <v>8</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B285" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D285" s="31" t="s">
-        <v>970</v>
+        <v>964</v>
       </c>
       <c r="E285" s="31" t="s">
-        <v>1007</v>
+        <v>1001</v>
       </c>
       <c r="G285" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I285" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="286" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B286" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D286" s="31" t="s">
+        <v>965</v>
+      </c>
+      <c r="E286" s="31" t="s">
+        <v>1002</v>
+      </c>
+      <c r="G286" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I286" s="4">
+        <v>9600</v>
+      </c>
+    </row>
+    <row r="287" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B287" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D287" s="31" t="s">
+        <v>966</v>
+      </c>
+      <c r="E287" s="31" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G287" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I287" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="288" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B288" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D288" s="31" t="s">
+        <v>967</v>
+      </c>
+      <c r="E288" s="31" t="s">
+        <v>1004</v>
+      </c>
+      <c r="G288" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I288" s="4">
         <v>1200</v>
-      </c>
-    </row>
-    <row r="286" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A286" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="B286" s="47" t="s">
-        <v>729</v>
-      </c>
-      <c r="C286" s="47" t="s">
-        <v>729</v>
-      </c>
-      <c r="D286" s="47" t="s">
-        <v>729</v>
-      </c>
-      <c r="E286" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="I286" s="49"/>
-      <c r="J286" s="49"/>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B287" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D287" s="31" t="s">
-        <v>914</v>
-      </c>
-      <c r="E287" s="31" t="s">
-        <v>707</v>
-      </c>
-      <c r="G287" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I287" s="4" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B288" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D288" s="31" t="s">
-        <v>915</v>
-      </c>
-      <c r="E288" s="31" t="s">
-        <v>894</v>
-      </c>
-      <c r="G288" s="31" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
@@ -13705,16 +13708,16 @@
         <v>21</v>
       </c>
       <c r="D289" s="31" t="s">
-        <v>1079</v>
+        <v>968</v>
       </c>
       <c r="E289" s="31" t="s">
-        <v>923</v>
+        <v>1005</v>
       </c>
       <c r="G289" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I289" s="4" t="s">
-        <v>916</v>
+        <v>64</v>
+      </c>
+      <c r="I289" s="4">
+        <v>9600</v>
       </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
@@ -13722,16 +13725,16 @@
         <v>21</v>
       </c>
       <c r="D290" s="31" t="s">
-        <v>1078</v>
+        <v>969</v>
       </c>
       <c r="E290" s="31" t="s">
-        <v>920</v>
+        <v>1006</v>
       </c>
       <c r="G290" s="31" t="s">
         <v>64</v>
       </c>
       <c r="I290" s="4">
-        <v>0.78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:10" x14ac:dyDescent="0.25">
@@ -13739,86 +13742,83 @@
         <v>21</v>
       </c>
       <c r="D291" s="31" t="s">
-        <v>1077</v>
+        <v>970</v>
       </c>
       <c r="E291" s="31" t="s">
-        <v>921</v>
+        <v>1007</v>
       </c>
       <c r="G291" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I291" s="4" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B292" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D292" s="31" t="s">
-        <v>1076</v>
-      </c>
-      <c r="E292" s="31" t="s">
-        <v>922</v>
-      </c>
-      <c r="G292" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I292" s="4">
-        <v>120</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="I291" s="4">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A292" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B292" s="47" t="s">
+        <v>729</v>
+      </c>
+      <c r="C292" s="47" t="s">
+        <v>729</v>
+      </c>
+      <c r="D292" s="47" t="s">
+        <v>729</v>
+      </c>
+      <c r="E292" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I292" s="49"/>
+      <c r="J292" s="49"/>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B293" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D293" s="31" t="s">
-        <v>1080</v>
+        <v>914</v>
       </c>
       <c r="E293" s="31" t="s">
-        <v>943</v>
+        <v>707</v>
       </c>
       <c r="G293" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I293" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="294" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A294" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="B294" s="47" t="s">
-        <v>1090</v>
-      </c>
-      <c r="C294" s="47" t="s">
-        <v>1090</v>
-      </c>
-      <c r="D294" s="47" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E294" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="I294" s="49"/>
-      <c r="J294" s="49"/>
+        <v>62</v>
+      </c>
+      <c r="I293" s="4" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B294" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D294" s="31" t="s">
+        <v>915</v>
+      </c>
+      <c r="E294" s="31" t="s">
+        <v>894</v>
+      </c>
+      <c r="G294" s="31" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B295" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D295" s="31" t="s">
-        <v>914</v>
+        <v>1079</v>
       </c>
       <c r="E295" s="31" t="s">
-        <v>707</v>
+        <v>923</v>
       </c>
       <c r="G295" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I295" s="4" t="s">
-        <v>853</v>
+        <v>916</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
@@ -13826,13 +13826,16 @@
         <v>21</v>
       </c>
       <c r="D296" s="31" t="s">
-        <v>915</v>
+        <v>1078</v>
       </c>
       <c r="E296" s="31" t="s">
-        <v>894</v>
+        <v>920</v>
       </c>
       <c r="G296" s="31" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="I296" s="4">
+        <v>0.78</v>
       </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
@@ -13840,16 +13843,16 @@
         <v>21</v>
       </c>
       <c r="D297" s="31" t="s">
-        <v>1093</v>
+        <v>1077</v>
       </c>
       <c r="E297" s="31" t="s">
-        <v>1091</v>
+        <v>921</v>
       </c>
       <c r="G297" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I297" s="4">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="I297" s="4" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
@@ -13857,100 +13860,100 @@
         <v>21</v>
       </c>
       <c r="D298" s="31" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="E298" s="31" t="s">
-        <v>1092</v>
+        <v>922</v>
       </c>
       <c r="G298" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I298" s="4" t="s">
-        <v>1050</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A299" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="B299" s="47" t="s">
-        <v>1094</v>
-      </c>
-      <c r="C299" s="47" t="s">
-        <v>1094</v>
-      </c>
-      <c r="D299" s="47" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E299" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="I298" s="4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B299" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D299" s="31" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E299" s="31" t="s">
+        <v>943</v>
+      </c>
+      <c r="G299" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I299" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A300" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B300" s="47" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C300" s="47" t="s">
+        <v>1090</v>
+      </c>
+      <c r="D300" s="47" t="s">
+        <v>1090</v>
+      </c>
+      <c r="E300" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="I299" s="49"/>
-      <c r="J299" s="49"/>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B300" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D300" s="31" t="s">
-        <v>914</v>
-      </c>
-      <c r="E300" s="31" t="s">
-        <v>707</v>
-      </c>
-      <c r="G300" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I300" s="4" t="s">
-        <v>853</v>
-      </c>
+      <c r="I300" s="49"/>
+      <c r="J300" s="49"/>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B301" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D301" s="31" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="E301" s="31" t="s">
-        <v>894</v>
+        <v>707</v>
       </c>
       <c r="G301" s="31" t="s">
         <v>62</v>
       </c>
+      <c r="I301" s="4" t="s">
+        <v>853</v>
+      </c>
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B302" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D302" s="31" t="s">
-        <v>1104</v>
+        <v>915</v>
       </c>
       <c r="E302" s="31" t="s">
-        <v>1096</v>
+        <v>894</v>
       </c>
       <c r="G302" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I302" s="4" t="s">
-        <v>1099</v>
-      </c>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B303" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D303" s="31" t="s">
-        <v>1105</v>
+        <v>1093</v>
       </c>
       <c r="E303" s="31" t="s">
-        <v>1097</v>
+        <v>1091</v>
       </c>
       <c r="G303" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I303" s="4" t="s">
-        <v>1050</v>
+        <v>64</v>
+      </c>
+      <c r="I303" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
@@ -13958,16 +13961,16 @@
         <v>21</v>
       </c>
       <c r="D304" s="31" t="s">
-        <v>1106</v>
+        <v>1077</v>
       </c>
       <c r="E304" s="31" t="s">
-        <v>1098</v>
+        <v>1092</v>
       </c>
       <c r="G304" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I304" s="4" t="s">
-        <v>1110</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="305" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -13975,16 +13978,16 @@
         <v>0</v>
       </c>
       <c r="B305" s="47" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="C305" s="47" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D305" s="47" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E305" s="48" t="s">
-        <v>160</v>
+        <v>68</v>
       </c>
       <c r="I305" s="49"/>
       <c r="J305" s="49"/>
@@ -14011,16 +14014,13 @@
         <v>21</v>
       </c>
       <c r="D307" s="31" t="s">
-        <v>1107</v>
+        <v>915</v>
       </c>
       <c r="E307" s="31" t="s">
-        <v>1100</v>
+        <v>894</v>
       </c>
       <c r="G307" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I307" s="4">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="308" spans="1:10" x14ac:dyDescent="0.25">
@@ -14028,16 +14028,16 @@
         <v>21</v>
       </c>
       <c r="D308" s="31" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="E308" s="31" t="s">
-        <v>1101</v>
+        <v>1096</v>
       </c>
       <c r="G308" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I308" s="4">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="I308" s="4" t="s">
+        <v>1099</v>
       </c>
     </row>
     <row r="309" spans="1:10" x14ac:dyDescent="0.25">
@@ -14045,16 +14045,16 @@
         <v>21</v>
       </c>
       <c r="D309" s="31" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="E309" s="31" t="s">
-        <v>1102</v>
+        <v>1097</v>
       </c>
       <c r="G309" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I309" s="4" t="b">
-        <v>0</v>
+        <v>62</v>
+      </c>
+      <c r="I309" s="4" t="s">
+        <v>1050</v>
       </c>
     </row>
     <row r="310" spans="1:10" x14ac:dyDescent="0.25">
@@ -14062,16 +14062,16 @@
         <v>21</v>
       </c>
       <c r="D310" s="31" t="s">
-        <v>1111</v>
+        <v>1106</v>
       </c>
       <c r="E310" s="31" t="s">
-        <v>1103</v>
+        <v>1098</v>
       </c>
       <c r="G310" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I310" s="4">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="I310" s="4" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="311" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -14079,16 +14079,16 @@
         <v>0</v>
       </c>
       <c r="B311" s="47" t="s">
-        <v>730</v>
+        <v>1095</v>
       </c>
       <c r="C311" s="47" t="s">
-        <v>730</v>
+        <v>1095</v>
       </c>
       <c r="D311" s="47" t="s">
-        <v>730</v>
+        <v>1095</v>
       </c>
       <c r="E311" s="48" t="s">
-        <v>68</v>
+        <v>160</v>
       </c>
       <c r="I311" s="49"/>
       <c r="J311" s="49"/>
@@ -14115,13 +14115,16 @@
         <v>21</v>
       </c>
       <c r="D313" s="31" t="s">
-        <v>915</v>
+        <v>1107</v>
       </c>
       <c r="E313" s="31" t="s">
-        <v>894</v>
+        <v>1100</v>
       </c>
       <c r="G313" s="31" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="I313" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:10" x14ac:dyDescent="0.25">
@@ -14129,16 +14132,16 @@
         <v>21</v>
       </c>
       <c r="D314" s="31" t="s">
-        <v>1082</v>
+        <v>1108</v>
       </c>
       <c r="E314" s="31" t="s">
-        <v>917</v>
+        <v>1101</v>
       </c>
       <c r="G314" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I314" s="4" t="s">
-        <v>919</v>
+        <v>64</v>
+      </c>
+      <c r="I314" s="4">
+        <v>55</v>
       </c>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
@@ -14146,69 +14149,69 @@
         <v>21</v>
       </c>
       <c r="D315" s="31" t="s">
-        <v>1081</v>
+        <v>1109</v>
       </c>
       <c r="E315" s="31" t="s">
-        <v>918</v>
+        <v>1102</v>
       </c>
       <c r="G315" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I315" s="4" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A316" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="B316" s="47" t="s">
-        <v>736</v>
-      </c>
-      <c r="C316" s="47" t="s">
-        <v>832</v>
-      </c>
-      <c r="D316" s="47" t="s">
-        <v>832</v>
-      </c>
-      <c r="E316" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="I315" s="4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B316" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D316" s="31" t="s">
+        <v>1111</v>
+      </c>
+      <c r="E316" s="31" t="s">
+        <v>1103</v>
+      </c>
+      <c r="G316" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I316" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A317" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B317" s="47" t="s">
+        <v>730</v>
+      </c>
+      <c r="C317" s="47" t="s">
+        <v>730</v>
+      </c>
+      <c r="D317" s="47" t="s">
+        <v>730</v>
+      </c>
+      <c r="E317" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="I316" s="49"/>
-      <c r="J316" s="49"/>
-    </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B317" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D317" s="31" t="s">
-        <v>787</v>
-      </c>
-      <c r="E317" s="31" t="s">
-        <v>807</v>
-      </c>
-      <c r="G317" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I317" s="4" t="s">
-        <v>1048</v>
-      </c>
+      <c r="I317" s="49"/>
+      <c r="J317" s="49"/>
     </row>
     <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B318" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D318" s="31" t="s">
-        <v>788</v>
+        <v>914</v>
       </c>
       <c r="E318" s="31" t="s">
-        <v>808</v>
+        <v>707</v>
       </c>
       <c r="G318" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I318" s="4" t="b">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="I318" s="4" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="319" spans="1:10" x14ac:dyDescent="0.25">
@@ -14216,129 +14219,128 @@
         <v>21</v>
       </c>
       <c r="D319" s="31" t="s">
-        <v>789</v>
+        <v>915</v>
       </c>
       <c r="E319" s="31" t="s">
-        <v>809</v>
+        <v>894</v>
       </c>
       <c r="G319" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I319" s="4">
-        <v>3</v>
-      </c>
     </row>
     <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B320" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D320" s="31" t="s">
-        <v>790</v>
+        <v>1082</v>
       </c>
       <c r="E320" s="31" t="s">
-        <v>810</v>
+        <v>917</v>
       </c>
       <c r="G320" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I320" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="I320" s="4" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B321" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D321" s="31" t="s">
-        <v>791</v>
+        <v>1081</v>
       </c>
       <c r="E321" s="31" t="s">
-        <v>811</v>
+        <v>918</v>
       </c>
       <c r="G321" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I321" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B322" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D322" s="31" t="s">
-        <v>792</v>
-      </c>
-      <c r="E322" s="31" t="s">
-        <v>812</v>
-      </c>
-      <c r="G322" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I322" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="323" spans="2:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="I321" s="4" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A322" s="47" t="b">
+        <v>0</v>
+      </c>
+      <c r="B322" s="47" t="s">
+        <v>736</v>
+      </c>
+      <c r="C322" s="47" t="s">
+        <v>832</v>
+      </c>
+      <c r="D322" s="47" t="s">
+        <v>832</v>
+      </c>
+      <c r="E322" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="I322" s="49"/>
+      <c r="J322" s="49"/>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B323" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D323" s="31" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
       <c r="E323" s="31" t="s">
-        <v>813</v>
+        <v>807</v>
       </c>
       <c r="G323" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I323" s="4" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.25">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B324" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D324" s="31" t="s">
-        <v>794</v>
+        <v>788</v>
       </c>
       <c r="E324" s="31" t="s">
-        <v>814</v>
+        <v>808</v>
       </c>
       <c r="G324" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I324" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="I324" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B325" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D325" s="31" t="s">
-        <v>795</v>
+        <v>789</v>
       </c>
       <c r="E325" s="31" t="s">
-        <v>815</v>
+        <v>809</v>
       </c>
       <c r="G325" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I325" s="4" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="I325" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B326" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D326" s="31" t="s">
-        <v>796</v>
+        <v>790</v>
       </c>
       <c r="E326" s="31" t="s">
-        <v>816</v>
+        <v>810</v>
       </c>
       <c r="G326" s="31" t="s">
         <v>64</v>
@@ -14347,173 +14349,275 @@
         <v>10</v>
       </c>
     </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B327" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D327" s="31" t="s">
+        <v>791</v>
+      </c>
+      <c r="E327" s="31" t="s">
+        <v>811</v>
+      </c>
+      <c r="G327" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I327" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B328" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D328" s="31" t="s">
+        <v>792</v>
+      </c>
+      <c r="E328" s="31" t="s">
+        <v>812</v>
+      </c>
+      <c r="G328" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I328" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B329" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D329" s="31" t="s">
+        <v>793</v>
+      </c>
+      <c r="E329" s="31" t="s">
+        <v>813</v>
+      </c>
+      <c r="G329" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I329" s="4" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B330" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D330" s="31" t="s">
+        <v>794</v>
+      </c>
+      <c r="E330" s="31" t="s">
+        <v>814</v>
+      </c>
+      <c r="G330" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I330" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B331" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D331" s="31" t="s">
+        <v>795</v>
+      </c>
+      <c r="E331" s="31" t="s">
+        <v>815</v>
+      </c>
+      <c r="G331" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I331" s="4" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B332" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D332" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="E332" s="31" t="s">
+        <v>816</v>
+      </c>
+      <c r="G332" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I332" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B333" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D333" s="31" t="s">
         <v>797</v>
       </c>
-      <c r="E327" s="31" t="s">
+      <c r="E333" s="31" t="s">
         <v>817</v>
-      </c>
-      <c r="G327" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I327" s="4" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B328" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D328" s="31" t="s">
-        <v>798</v>
-      </c>
-      <c r="E328" s="31" t="s">
-        <v>818</v>
-      </c>
-      <c r="G328" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I328" s="4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="329" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B329" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D329" s="31" t="s">
-        <v>799</v>
-      </c>
-      <c r="E329" s="31" t="s">
-        <v>819</v>
-      </c>
-      <c r="G329" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I329" s="4">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="330" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B330" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D330" s="31" t="s">
-        <v>800</v>
-      </c>
-      <c r="E330" s="31" t="s">
-        <v>820</v>
-      </c>
-      <c r="G330" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I330" s="4">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="331" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B331" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D331" s="31" t="s">
-        <v>801</v>
-      </c>
-      <c r="E331" s="31" t="s">
-        <v>821</v>
-      </c>
-      <c r="G331" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="I331" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B332" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D332" s="31" t="s">
-        <v>802</v>
-      </c>
-      <c r="E332" s="31" t="s">
-        <v>822</v>
-      </c>
-      <c r="G332" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="I332" s="4" t="s">
-        <v>828</v>
-      </c>
-    </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B333" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D333" s="31" t="s">
-        <v>803</v>
-      </c>
-      <c r="E333" s="31" t="s">
-        <v>825</v>
       </c>
       <c r="G333" s="31" t="s">
         <v>62</v>
       </c>
       <c r="I333" s="4" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B334" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D334" s="31" t="s">
+        <v>798</v>
+      </c>
+      <c r="E334" s="31" t="s">
+        <v>818</v>
+      </c>
+      <c r="G334" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I334" s="4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B335" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D335" s="31" t="s">
+        <v>799</v>
+      </c>
+      <c r="E335" s="31" t="s">
+        <v>819</v>
+      </c>
+      <c r="G335" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I335" s="4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B336" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D336" s="31" t="s">
+        <v>800</v>
+      </c>
+      <c r="E336" s="31" t="s">
+        <v>820</v>
+      </c>
+      <c r="G336" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I336" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="337" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B337" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D337" s="31" t="s">
+        <v>801</v>
+      </c>
+      <c r="E337" s="31" t="s">
+        <v>821</v>
+      </c>
+      <c r="G337" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I337" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B338" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D338" s="31" t="s">
+        <v>802</v>
+      </c>
+      <c r="E338" s="31" t="s">
+        <v>822</v>
+      </c>
+      <c r="G338" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I338" s="4" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="339" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B339" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D339" s="31" t="s">
+        <v>803</v>
+      </c>
+      <c r="E339" s="31" t="s">
+        <v>825</v>
+      </c>
+      <c r="G339" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I339" s="4" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="334" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B334" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D334" s="31" t="s">
+    <row r="340" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B340" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D340" s="31" t="s">
         <v>804</v>
       </c>
-      <c r="E334" s="31" t="s">
+      <c r="E340" s="31" t="s">
         <v>823</v>
       </c>
-      <c r="G334" s="31" t="s">
+      <c r="G340" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I334" s="4" t="s">
+      <c r="I340" s="4" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="335" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B335" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D335" s="31" t="s">
+    <row r="341" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B341" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D341" s="31" t="s">
         <v>805</v>
       </c>
-      <c r="E335" s="31" t="s">
+      <c r="E341" s="31" t="s">
         <v>824</v>
       </c>
-      <c r="G335" s="31" t="s">
+      <c r="G341" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="I335" s="4" t="s">
+      <c r="I341" s="4" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="336" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B336" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="D336" s="31" t="s">
+    <row r="342" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B342" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D342" s="31" t="s">
         <v>806</v>
       </c>
-      <c r="E336" s="31" t="s">
+      <c r="E342" s="31" t="s">
         <v>826</v>
       </c>
-      <c r="G336" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="I336" s="4">
+      <c r="G342" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="I342" s="4">
         <v>0</v>
       </c>
     </row>
@@ -14541,7 +14645,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23824,8 +23928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>